<commit_message>
Updating to current design.
Please note, all the STLs and 3MFs require reproducing
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -3046,9 +3046,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{B1CD5D04-AD61-4709-BF60-EFC62F156AF5}" name="James Skitt" id="-1400019162" dateTime="2019-11-15T09:54:41"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>